<commit_message>
Added lesson 22. Greetings
</commit_message>
<xml_diff>
--- a/Zhodani Words List.xlsx
+++ b/Zhodani Words List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkaz1\Documents\GitHub\Zdetl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CBDD1B-73BB-4148-B5E9-9A2BCFBDCEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D0893A-9BFB-4952-8F51-890D29FB196D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{06097C92-1E44-4EB6-8222-C9DA7786637A}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2251" uniqueCount="975">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2259" uniqueCount="976">
   <si>
     <t>Zhdetl word</t>
   </si>
@@ -2998,6 +2998,9 @@
   </si>
   <si>
     <t>good night</t>
+  </si>
+  <si>
+    <t>22. Greetings</t>
   </si>
 </sst>
 </file>
@@ -3166,6 +3169,16 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -3194,16 +3207,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3236,8 +3239,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B4039E8B-8AC1-44D4-939F-61521D537543}" name="Zhdetl" displayName="Zhdetl" ref="A1:B186" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B186" xr:uid="{B2E9EE69-E126-4FC1-ACEF-C598B63AECDE}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{5FF4A609-EB29-4591-80AA-89AF1E219E8F}" uniqueName="1" name="Word" queryTableFieldId="1" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{7D4C4436-96EC-4C21-A85D-7C6AE2F8E895}" uniqueName="2" name="Meaning" queryTableFieldId="2" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{5FF4A609-EB29-4591-80AA-89AF1E219E8F}" uniqueName="1" name="Word" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{7D4C4436-96EC-4C21-A85D-7C6AE2F8E895}" uniqueName="2" name="Meaning" queryTableFieldId="2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6224,8 +6227,8 @@
   <dimension ref="A1:C551"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <pane ySplit="1" topLeftCell="A306" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B318" sqref="B318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6872,7 +6875,9 @@
       <c r="A63" s="17" t="s">
         <v>965</v>
       </c>
-      <c r="B63" s="21"/>
+      <c r="B63" s="21" t="s">
+        <v>975</v>
+      </c>
       <c r="C63" s="18" t="s">
         <v>966</v>
       </c>
@@ -6890,7 +6895,9 @@
       <c r="A65" s="17" t="s">
         <v>967</v>
       </c>
-      <c r="B65" s="21"/>
+      <c r="B65" s="21" t="s">
+        <v>975</v>
+      </c>
       <c r="C65" s="18" t="s">
         <v>968</v>
       </c>
@@ -8703,7 +8710,9 @@
       <c r="A242" s="14" t="s">
         <v>959</v>
       </c>
-      <c r="B242" s="14"/>
+      <c r="B242" s="14" t="s">
+        <v>975</v>
+      </c>
       <c r="C242" s="25" t="s">
         <v>960</v>
       </c>
@@ -8712,7 +8721,9 @@
       <c r="A243" s="14" t="s">
         <v>961</v>
       </c>
-      <c r="B243" s="14"/>
+      <c r="B243" s="14" t="s">
+        <v>975</v>
+      </c>
       <c r="C243" s="14" t="s">
         <v>962</v>
       </c>
@@ -8721,7 +8732,9 @@
       <c r="A244" s="14" t="s">
         <v>963</v>
       </c>
-      <c r="B244" s="14"/>
+      <c r="B244" s="14" t="s">
+        <v>975</v>
+      </c>
       <c r="C244" s="14" t="s">
         <v>964</v>
       </c>
@@ -9452,7 +9465,9 @@
       <c r="A317" s="14" t="s">
         <v>973</v>
       </c>
-      <c r="B317" s="14"/>
+      <c r="B317" s="14" t="s">
+        <v>975</v>
+      </c>
       <c r="C317" s="14" t="s">
         <v>974</v>
       </c>
@@ -9598,7 +9613,9 @@
       <c r="A331" s="14" t="s">
         <v>969</v>
       </c>
-      <c r="B331" s="14"/>
+      <c r="B331" s="14" t="s">
+        <v>975</v>
+      </c>
       <c r="C331" s="14" t="s">
         <v>970</v>
       </c>
@@ -9748,7 +9765,9 @@
       <c r="A345" s="14" t="s">
         <v>971</v>
       </c>
-      <c r="B345" s="14"/>
+      <c r="B345" s="14" t="s">
+        <v>975</v>
+      </c>
       <c r="C345" s="14" t="s">
         <v>972</v>
       </c>
@@ -11083,13 +11102,13 @@
   </sortState>
   <dataConsolidate/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A375:A1048576 A372:A373 A259:A370 A192:A257 A1:A190">
-    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="9"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated list with boolean terms
</commit_message>
<xml_diff>
--- a/Zhodani Words List.xlsx
+++ b/Zhodani Words List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkaz1\Documents\GitHub\Zdetl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06385F46-C376-4B5C-8077-8D3AF49DA377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FFDF7A-84CE-46B2-8782-C17FCAC2FB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{06097C92-1E44-4EB6-8222-C9DA7786637A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{06097C92-1E44-4EB6-8222-C9DA7786637A}"/>
   </bookViews>
   <sheets>
     <sheet name="Lessons" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Current vocabulary list'!$A$1:$C$457</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Current vocabulary list'!$A$1:$C$450</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lessons!$A$1:$C$223</definedName>
     <definedName name="ExternalData_1" localSheetId="2" hidden="1">'Zhdetl (from Alien Book 4)'!$A$1:$B$186</definedName>
   </definedNames>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2262" uniqueCount="978">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2283" uniqueCount="992">
   <si>
     <t>Zhdetl word</t>
   </si>
@@ -3007,6 +3007,48 @@
   </si>
   <si>
     <t>greeter; night-time greeter</t>
+  </si>
+  <si>
+    <t>23. Truth and Falsehood</t>
+  </si>
+  <si>
+    <t>iazh</t>
+  </si>
+  <si>
+    <t>pra</t>
+  </si>
+  <si>
+    <t>shti</t>
+  </si>
+  <si>
+    <t>falsehood; can also mean 'no' depeding on context</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'and', meaning both or all conditions are true</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'or', meaining either condition can be true</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'not', implying that either an expression is false or a comparision is false (as in A but not B)</t>
+  </si>
+  <si>
+    <t>plaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'xor', or 'either one or the other but not both, used when there are several choices that cannot be simultaneously true</t>
+  </si>
+  <si>
+    <t>chapra</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'nor', both or all conditions are not true</t>
+  </si>
+  <si>
+    <t>plachapra</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'xnor', both or all conditions are true or false</t>
   </si>
 </sst>
 </file>
@@ -6230,11 +6272,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C2C8BF-DF2D-49AF-9216-32C7AE890ACB}">
-  <dimension ref="A1:C552"/>
+  <dimension ref="A1:C542"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A306" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A318" sqref="A318"/>
+      <pane ySplit="1" topLeftCell="A442" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A455" sqref="A455"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10809,39 +10851,81 @@
       </c>
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A448" s="14"/>
-      <c r="B448" s="14"/>
-      <c r="C448" s="14"/>
+      <c r="A448" s="14" t="s">
+        <v>979</v>
+      </c>
+      <c r="B448" s="14" t="s">
+        <v>978</v>
+      </c>
+      <c r="C448" s="25" t="s">
+        <v>983</v>
+      </c>
     </row>
     <row r="449" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A449" s="14"/>
-      <c r="B449" s="14"/>
-      <c r="C449" s="14"/>
+      <c r="A449" s="14" t="s">
+        <v>980</v>
+      </c>
+      <c r="B449" s="14" t="s">
+        <v>978</v>
+      </c>
+      <c r="C449" s="25" t="s">
+        <v>984</v>
+      </c>
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A450" s="14"/>
-      <c r="B450" s="14"/>
-      <c r="C450" s="14"/>
+      <c r="A450" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B450" s="14" t="s">
+        <v>978</v>
+      </c>
+      <c r="C450" s="14" t="s">
+        <v>982</v>
+      </c>
     </row>
     <row r="451" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A451" s="14"/>
-      <c r="B451" s="14"/>
-      <c r="C451" s="14"/>
+      <c r="A451" s="14" t="s">
+        <v>981</v>
+      </c>
+      <c r="B451" s="14" t="s">
+        <v>978</v>
+      </c>
+      <c r="C451" s="25" t="s">
+        <v>985</v>
+      </c>
     </row>
     <row r="452" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A452" s="14"/>
-      <c r="B452" s="14"/>
-      <c r="C452" s="14"/>
+      <c r="A452" s="14" t="s">
+        <v>986</v>
+      </c>
+      <c r="B452" s="14" t="s">
+        <v>978</v>
+      </c>
+      <c r="C452" s="14" t="s">
+        <v>987</v>
+      </c>
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A453" s="14"/>
-      <c r="B453" s="14"/>
-      <c r="C453" s="14"/>
+      <c r="A453" s="14" t="s">
+        <v>988</v>
+      </c>
+      <c r="B453" s="14" t="s">
+        <v>978</v>
+      </c>
+      <c r="C453" s="14" t="s">
+        <v>989</v>
+      </c>
     </row>
     <row r="454" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A454" s="14"/>
-      <c r="B454" s="14"/>
-      <c r="C454" s="14"/>
+      <c r="A454" s="14" t="s">
+        <v>990</v>
+      </c>
+      <c r="B454" s="14" t="s">
+        <v>978</v>
+      </c>
+      <c r="C454" s="14" t="s">
+        <v>991</v>
+      </c>
     </row>
     <row r="455" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A455" s="14"/>
@@ -10859,9 +10943,9 @@
       <c r="C457" s="14"/>
     </row>
     <row r="458" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A458" s="14"/>
-      <c r="B458" s="14"/>
-      <c r="C458" s="25"/>
+      <c r="A458" s="25"/>
+      <c r="B458" s="25"/>
+      <c r="C458" s="14"/>
     </row>
     <row r="459" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A459" s="14"/>
@@ -10876,7 +10960,7 @@
     <row r="461" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A461" s="14"/>
       <c r="B461" s="14"/>
-      <c r="C461" s="25"/>
+      <c r="C461" s="14"/>
     </row>
     <row r="462" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A462" s="14"/>
@@ -10909,8 +10993,8 @@
       <c r="C467" s="14"/>
     </row>
     <row r="468" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A468" s="25"/>
-      <c r="B468" s="25"/>
+      <c r="A468" s="14"/>
+      <c r="B468" s="14"/>
       <c r="C468" s="14"/>
     </row>
     <row r="469" spans="1:3" x14ac:dyDescent="0.3">
@@ -10966,156 +11050,106 @@
     <row r="479" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A479" s="14"/>
       <c r="B479" s="14"/>
-      <c r="C479" s="14"/>
+      <c r="C479" s="25"/>
     </row>
     <row r="480" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A480" s="14"/>
       <c r="B480" s="14"/>
-      <c r="C480" s="14"/>
+      <c r="C480" s="13"/>
     </row>
     <row r="481" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A481" s="14"/>
       <c r="B481" s="14"/>
-      <c r="C481" s="14"/>
+      <c r="C481" s="13"/>
     </row>
     <row r="482" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A482" s="14"/>
-      <c r="B482" s="14"/>
-      <c r="C482" s="14"/>
+      <c r="A482" s="11"/>
+      <c r="B482" s="11"/>
+      <c r="C482" s="12"/>
     </row>
     <row r="483" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A483" s="14"/>
       <c r="B483" s="14"/>
       <c r="C483" s="14"/>
     </row>
-    <row r="484" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A484" s="14"/>
-      <c r="B484" s="14"/>
-      <c r="C484" s="14"/>
-    </row>
-    <row r="485" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A485" s="14"/>
-      <c r="B485" s="14"/>
-      <c r="C485" s="14"/>
-    </row>
-    <row r="486" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A486" s="14"/>
-      <c r="B486" s="14"/>
-      <c r="C486" s="14"/>
-    </row>
-    <row r="487" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A487" s="14"/>
-      <c r="B487" s="14"/>
-      <c r="C487" s="14"/>
-    </row>
-    <row r="488" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A488" s="14"/>
-      <c r="B488" s="14"/>
-      <c r="C488" s="14"/>
-    </row>
-    <row r="489" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A489" s="14"/>
-      <c r="B489" s="14"/>
-      <c r="C489" s="25"/>
-    </row>
-    <row r="490" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B490" s="14"/>
-      <c r="C490" s="13"/>
-    </row>
-    <row r="491" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B491" s="14"/>
-      <c r="C491" s="13"/>
-    </row>
     <row r="492" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A492" s="11"/>
-      <c r="B492" s="11"/>
-      <c r="C492" s="12"/>
-    </row>
-    <row r="493" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A493" s="14"/>
-      <c r="B493" s="14"/>
-      <c r="C493" s="14"/>
-    </row>
-    <row r="502" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C502" s="13"/>
-    </row>
-    <row r="504" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A504" s="13"/>
-      <c r="B504" s="13"/>
-    </row>
-    <row r="505" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C505" s="13"/>
-    </row>
-    <row r="522" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C522" s="13"/>
+      <c r="C492" s="13"/>
+    </row>
+    <row r="494" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A494" s="13"/>
+      <c r="B494" s="13"/>
+    </row>
+    <row r="495" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C495" s="13"/>
+    </row>
+    <row r="512" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C512" s="13"/>
+    </row>
+    <row r="528" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C528" s="13"/>
+    </row>
+    <row r="529" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A529" s="14"/>
+      <c r="B529" s="14"/>
+      <c r="C529" s="14"/>
+    </row>
+    <row r="530" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A530" s="11"/>
+      <c r="B530" s="11"/>
+      <c r="C530" s="12"/>
+    </row>
+    <row r="531" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A531" s="14"/>
+      <c r="B531" s="14"/>
+      <c r="C531" s="14"/>
+    </row>
+    <row r="532" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A532" s="14"/>
+      <c r="B532" s="14"/>
+      <c r="C532" s="14"/>
+    </row>
+    <row r="533" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A533" s="14"/>
+      <c r="B533" s="14"/>
+      <c r="C533" s="14"/>
+    </row>
+    <row r="534" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A534" s="14"/>
+      <c r="B534" s="14"/>
+      <c r="C534" s="14"/>
+    </row>
+    <row r="535" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A535" s="14"/>
+      <c r="B535" s="14"/>
+      <c r="C535" s="14"/>
+    </row>
+    <row r="536" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A536" s="14"/>
+      <c r="B536" s="14"/>
+      <c r="C536" s="14"/>
+    </row>
+    <row r="537" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A537" s="14"/>
+      <c r="B537" s="14"/>
+      <c r="C537" s="14"/>
     </row>
     <row r="538" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C538" s="13"/>
+      <c r="A538" s="14"/>
+      <c r="B538" s="14"/>
+      <c r="C538" s="14"/>
     </row>
     <row r="539" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A539" s="14"/>
       <c r="B539" s="14"/>
       <c r="C539" s="14"/>
     </row>
-    <row r="540" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A540" s="11"/>
-      <c r="B540" s="11"/>
-      <c r="C540" s="12"/>
-    </row>
-    <row r="541" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A541" s="14"/>
-      <c r="B541" s="14"/>
-      <c r="C541" s="14"/>
-    </row>
     <row r="542" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A542" s="14"/>
       <c r="B542" s="14"/>
       <c r="C542" s="14"/>
     </row>
-    <row r="543" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A543" s="14"/>
-      <c r="B543" s="14"/>
-      <c r="C543" s="14"/>
-    </row>
-    <row r="544" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A544" s="14"/>
-      <c r="B544" s="14"/>
-      <c r="C544" s="14"/>
-    </row>
-    <row r="545" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A545" s="14"/>
-      <c r="B545" s="14"/>
-      <c r="C545" s="14"/>
-    </row>
-    <row r="546" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A546" s="14"/>
-      <c r="B546" s="14"/>
-      <c r="C546" s="14"/>
-    </row>
-    <row r="547" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A547" s="14"/>
-      <c r="B547" s="14"/>
-      <c r="C547" s="14"/>
-    </row>
-    <row r="548" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A548" s="14"/>
-      <c r="B548" s="14"/>
-      <c r="C548" s="14"/>
-    </row>
-    <row r="549" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A549" s="14"/>
-      <c r="B549" s="14"/>
-      <c r="C549" s="14"/>
-    </row>
-    <row r="552" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A552" s="14"/>
-      <c r="B552" s="14"/>
-      <c r="C552" s="14"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C457" xr:uid="{88C2C8BF-DF2D-49AF-9216-32C7AE890ACB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C552">
-    <sortCondition ref="A2:A552"/>
+  <autoFilter ref="A1:C450" xr:uid="{88C2C8BF-DF2D-49AF-9216-32C7AE890ACB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C542">
+    <sortCondition ref="A2:A542"/>
   </sortState>
   <dataConsolidate/>
   <conditionalFormatting sqref="C1:C1048576">
@@ -11136,8 +11170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{202BFE38-5763-453D-9FF5-A2457E37E84D}">
   <dimension ref="A1:B186"/>
   <sheetViews>
-    <sheetView topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B186"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>